<commit_message>
o hodně další verze
hodně změn
</commit_message>
<xml_diff>
--- a/grafy/fykos_res_analyzy.xlsx
+++ b/grafy/fykos_res_analyzy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8475"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8475" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Konec roku" sheetId="1" r:id="rId1"/>
@@ -692,7 +692,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -770,7 +770,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,7 +782,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="čárky" xfId="1" builtinId="3"/>
@@ -993,11 +994,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87087744"/>
-        <c:axId val="72208768"/>
+        <c:axId val="78629504"/>
+        <c:axId val="117817728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87087744"/>
+        <c:axId val="78629504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="27"/>
@@ -1016,12 +1017,12 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72208768"/>
+        <c:crossAx val="117817728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72208768"/>
+        <c:axId val="117817728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="210"/>
@@ -1041,7 +1042,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87087744"/>
+        <c:crossAx val="78629504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1240,23 +1241,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="72218880"/>
-        <c:axId val="125034496"/>
+        <c:axId val="117827840"/>
+        <c:axId val="118026240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72218880"/>
+        <c:axId val="117827840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125034496"/>
+        <c:crossAx val="118026240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125034496"/>
+        <c:axId val="118026240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,7 +1265,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72218880"/>
+        <c:crossAx val="117827840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1281,7 +1282,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12576613926828134"/>
+          <c:y val="3.631314900396606E-2"/>
+          <c:w val="0.8453951287438406"/>
+          <c:h val="0.79598718392680179"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -1298,11 +1309,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="66675">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:xVal>
             <c:numRef>
               <c:f>'Konec roku'!$A$3:$A$30</c:f>
@@ -1463,17 +1469,35 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="124883328"/>
-        <c:axId val="124884864"/>
+        <c:axId val="117866880"/>
+        <c:axId val="117868416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124883328"/>
+        <c:axId val="117866880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="27"/>
           <c:min val="12"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2200"/>
+                  <a:t>Ročník FYKOSu</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -1481,18 +1505,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600"/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124884864"/>
+        <c:crossAx val="117868416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124884864"/>
+        <c:axId val="117868416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1500,6 +1524,31 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2200"/>
+                  <a:t>Počet úspěšných řešitelů</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6372092543575387E-2"/>
+              <c:y val="0.19146260893030786"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -1507,12 +1556,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600"/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124883328"/>
+        <c:crossAx val="117866880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1529,7 +1578,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13844774299854015"/>
+          <c:y val="3.631314900396606E-2"/>
+          <c:w val="0.83271352501358153"/>
+          <c:h val="0.79598718392680179"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -1546,11 +1605,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="66675">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
           <c:xVal>
             <c:numRef>
               <c:f>'Konec roku'!$A$3:$A$30</c:f>
@@ -1648,7 +1702,7 @@
             <c:numRef>
               <c:f>'Konec roku'!$P$3:$P$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>0.10344827586206896</c:v>
@@ -1698,27 +1752,45 @@
                 <c:pt idx="15">
                   <c:v>9.580838323353294E-2</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="19" formatCode="0.0%">
                   <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="20" formatCode="0.0%">
                   <c:v>6.4516129032258063E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="124945536"/>
-        <c:axId val="124947072"/>
+        <c:axId val="117933184"/>
+        <c:axId val="117934720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124945536"/>
+        <c:axId val="117933184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="27"/>
           <c:min val="12"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2200"/>
+                  <a:t>Ročník FYKOSu</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -1726,18 +1798,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600"/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124947072"/>
+        <c:crossAx val="117934720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124947072"/>
+        <c:axId val="117934720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.14000000000000001"/>
@@ -1745,19 +1817,49 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2200"/>
+                  <a:t>Podíl počtu úspěšných řešitelů v </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="cs-CZ" sz="2200"/>
+                  <a:t>ročníku</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.7736433588873338E-2"/>
+              <c:y val="4.3376711595814472E-2"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600"/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124945536"/>
+        <c:crossAx val="117933184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1796,7 +1898,8 @@
     <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -1804,10 +1907,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -2206,9 +2310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2224,21 +2326,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:22">
       <c r="D2" s="3" t="s">
@@ -2332,7 +2434,7 @@
         <f>SUM(K3:N3)</f>
         <v>21</v>
       </c>
-      <c r="P3" s="43">
+      <c r="P3" s="44">
         <f t="shared" ref="P3" si="0">O3/H3</f>
         <v>0.10344827586206896</v>
       </c>
@@ -2389,11 +2491,11 @@
         <f>SUM(K4:N4)</f>
         <v>12</v>
       </c>
-      <c r="P4" s="43">
+      <c r="P4" s="44">
         <f t="shared" ref="P4:P18" si="1">O4/H4</f>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="R4" s="47">
+      <c r="R4" s="43">
         <f>AVERAGE(P3:P18)</f>
         <v>6.6348782734454173E-2</v>
       </c>
@@ -2445,7 +2547,7 @@
         <f>SUM(K5:N5)</f>
         <v>14</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="45">
         <f t="shared" si="1"/>
         <v>0.11475409836065574</v>
       </c>
@@ -2495,7 +2597,7 @@
         <f>SUM(K6:N6)</f>
         <v>1</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="45">
         <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
@@ -2549,7 +2651,7 @@
         <f>SUM(K7:N7)</f>
         <v>3</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="45">
         <f t="shared" si="1"/>
         <v>5.0847457627118647E-2</v>
       </c>
@@ -2599,7 +2701,7 @@
         <f t="shared" ref="O8:O21" si="3">SUM(K8:N8)</f>
         <v>2</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="45">
         <f t="shared" si="1"/>
         <v>2.9850746268656716E-2</v>
       </c>
@@ -2659,7 +2761,7 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="45">
         <f t="shared" si="1"/>
         <v>0.12987012987012986</v>
       </c>
@@ -2719,7 +2821,7 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="45">
         <f t="shared" si="1"/>
         <v>5.7971014492753624E-2</v>
       </c>
@@ -2779,7 +2881,7 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="45">
         <f t="shared" si="1"/>
         <v>7.2727272727272724E-2</v>
       </c>
@@ -2839,7 +2941,7 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="45">
         <f t="shared" si="1"/>
         <v>5.5555555555555552E-2</v>
       </c>
@@ -2899,7 +3001,7 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="45">
         <f t="shared" si="1"/>
         <v>1.6393442622950821E-2</v>
       </c>
@@ -2959,7 +3061,7 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14" s="45">
         <f t="shared" si="1"/>
         <v>5.6074766355140186E-2</v>
       </c>
@@ -3019,7 +3121,7 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="P15" s="1">
+      <c r="P15" s="45">
         <f t="shared" si="1"/>
         <v>6.9230769230769235E-2</v>
       </c>
@@ -3079,7 +3181,7 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="P16" s="1">
+      <c r="P16" s="45">
         <f t="shared" si="1"/>
         <v>3.9735099337748346E-2</v>
       </c>
@@ -3139,7 +3241,7 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17" s="45">
         <f t="shared" si="1"/>
         <v>8.1218274111675121E-2</v>
       </c>
@@ -3199,7 +3301,7 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="P18" s="1">
+      <c r="P18" s="45">
         <f t="shared" si="1"/>
         <v>9.580838323353294E-2</v>
       </c>
@@ -3458,14 +3560,14 @@
       <c r="C25" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="44">
+      <c r="D25" s="46">
         <v>110</v>
       </c>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44">
+      <c r="E25" s="46"/>
+      <c r="F25" s="46">
         <v>20</v>
       </c>
-      <c r="G25" s="44"/>
+      <c r="G25" s="46"/>
       <c r="H25" s="3">
         <f>F25+D25</f>
         <v>130</v>
@@ -3494,14 +3596,14 @@
       <c r="C26" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="44">
+      <c r="D26" s="46">
         <v>100</v>
       </c>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44">
+      <c r="E26" s="46"/>
+      <c r="F26" s="46">
         <v>40</v>
       </c>
-      <c r="G26" s="44"/>
+      <c r="G26" s="46"/>
       <c r="H26" s="3">
         <f>F26+D26</f>
         <v>140</v>
@@ -3530,14 +3632,14 @@
       <c r="C27" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="44">
+      <c r="D27" s="46">
         <v>80</v>
       </c>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44">
+      <c r="E27" s="46"/>
+      <c r="F27" s="46">
         <v>70</v>
       </c>
-      <c r="G27" s="44"/>
+      <c r="G27" s="46"/>
       <c r="H27" s="3">
         <f>F27+D27</f>
         <v>150</v>
@@ -4298,29 +4400,29 @@
       </c>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
       <c r="W11" s="5">
         <v>509938</v>
       </c>
@@ -4332,29 +4434,29 @@
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
       <c r="W12" s="5">
         <v>463349</v>
       </c>
@@ -4366,29 +4468,29 @@
       </c>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
       <c r="W13" s="5">
         <v>451070</v>
       </c>

</xml_diff>